<commit_message>
Updated relevant_markes.xlsx with two additional rs numbers, dbSNP export still needs to be refreshed
</commit_message>
<xml_diff>
--- a/knowledge-base/trunk/data/relevant-markers/relevant_markers.xlsx
+++ b/knowledge-base/trunk/data/relevant-markers/relevant_markers.xlsx
@@ -7,21 +7,22 @@
     <workbookView xWindow="360" yWindow="510" windowWidth="10710" windowHeight="5700" tabRatio="741"/>
   </bookViews>
   <sheets>
-    <sheet name="MERGED LIST " sheetId="18" r:id="rId1"/>
-    <sheet name="PharmADME core 02.2012" sheetId="2" r:id="rId2"/>
-    <sheet name="Information need PharmADME core" sheetId="4" r:id="rId3"/>
-    <sheet name="PharmGKB VIP 27.02.2012" sheetId="8" r:id="rId4"/>
-    <sheet name="PharmGKB Summary" sheetId="10" r:id="rId5"/>
-    <sheet name="FDA drug labels" sheetId="15" r:id="rId6"/>
-    <sheet name="PharmGKB PharmaADME merge" sheetId="17" r:id="rId7"/>
-    <sheet name="FDA additional RSID markers" sheetId="16" r:id="rId8"/>
-    <sheet name="Matthias Core SNP summary" sheetId="19" r:id="rId9"/>
+    <sheet name="Manual update 25.11.2013" sheetId="20" r:id="rId1"/>
+    <sheet name="MERGED LIST " sheetId="18" r:id="rId2"/>
+    <sheet name="PharmADME core 02.2012" sheetId="2" r:id="rId3"/>
+    <sheet name="Information need PharmADME core" sheetId="4" r:id="rId4"/>
+    <sheet name="PharmGKB VIP 27.02.2012" sheetId="8" r:id="rId5"/>
+    <sheet name="PharmGKB Summary" sheetId="10" r:id="rId6"/>
+    <sheet name="FDA drug labels" sheetId="15" r:id="rId7"/>
+    <sheet name="PharmGKB PharmaADME merge" sheetId="17" r:id="rId8"/>
+    <sheet name="FDA additional RSID markers" sheetId="16" r:id="rId9"/>
+    <sheet name="Matthias Core SNP summary" sheetId="19" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId10"/>
-    <pivotCache cacheId="1" r:id="rId11"/>
-    <pivotCache cacheId="2" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId11"/>
+    <pivotCache cacheId="1" r:id="rId12"/>
+    <pivotCache cacheId="2" r:id="rId13"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -112,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3932" uniqueCount="1290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4712" uniqueCount="1292">
   <si>
     <t>Gene</t>
   </si>
@@ -3982,6 +3983,12 @@
   </si>
   <si>
     <t>(blank)</t>
+  </si>
+  <si>
+    <t>rs67376798</t>
+  </si>
+  <si>
+    <t>rs2297595</t>
   </si>
 </sst>
 </file>
@@ -4109,7 +4116,37 @@
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4180,6 +4217,26 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -10637,6 +10694,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table103" displayName="Table103" ref="A1:C1048574" totalsRowShown="0">
+  <autoFilter ref="A1:C1048574"/>
+  <sortState ref="A2:C388">
+    <sortCondition ref="A1:A1048574"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" name="gene"/>
+    <tableColumn id="2" name="rsid"/>
+    <tableColumn id="3" name="comment"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:C1048574" totalsRowShown="0">
   <autoFilter ref="A1:C1048574"/>
   <sortState ref="A2:C388">
@@ -10651,8 +10723,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J186" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J186" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:J186">
     <filterColumn colId="4">
       <filters>
@@ -10803,22 +10875,22 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" name="Gene" dataDxfId="11"/>
-    <tableColumn id="2" name="Star Nomenclature" dataDxfId="10"/>
-    <tableColumn id="3" name="Nucloetide Change" dataDxfId="9"/>
-    <tableColumn id="4" name="Amino Acid Change" dataDxfId="8"/>
-    <tableColumn id="5" name="RS #" dataDxfId="7"/>
-    <tableColumn id="6" name="Build" dataDxfId="6"/>
-    <tableColumn id="7" name="Chromosome" dataDxfId="5"/>
-    <tableColumn id="8" name="Position" dataDxfId="4"/>
-    <tableColumn id="9" name="Upstream Sequence" dataDxfId="3"/>
-    <tableColumn id="10" name="Downstream Sequence" dataDxfId="2"/>
+    <tableColumn id="1" name="Gene" dataDxfId="14"/>
+    <tableColumn id="2" name="Star Nomenclature" dataDxfId="13"/>
+    <tableColumn id="3" name="Nucloetide Change" dataDxfId="12"/>
+    <tableColumn id="4" name="Amino Acid Change" dataDxfId="11"/>
+    <tableColumn id="5" name="RS #" dataDxfId="10"/>
+    <tableColumn id="6" name="Build" dataDxfId="9"/>
+    <tableColumn id="7" name="Chromosome" dataDxfId="8"/>
+    <tableColumn id="8" name="Position" dataDxfId="7"/>
+    <tableColumn id="9" name="Upstream Sequence" dataDxfId="6"/>
+    <tableColumn id="10" name="Downstream Sequence" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C322" totalsRowShown="0">
   <autoFilter ref="A1:C322"/>
   <tableColumns count="3">
@@ -10830,7 +10902,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:E1048576" totalsRowShown="0">
   <autoFilter ref="A1:E1048576"/>
   <tableColumns count="5">
@@ -11133,7 +11205,3686 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C388"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
+      <selection activeCell="L382" sqref="L382"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>760</v>
+      </c>
+      <c r="C1" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>840</v>
+      </c>
+      <c r="C2" s="15"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="15"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="15"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="15"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>841</v>
+      </c>
+      <c r="C6" s="15"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>842</v>
+      </c>
+      <c r="C7" s="15"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="15"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="15"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="15"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="15"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="15"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>761</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>762</v>
+      </c>
+      <c r="C16" s="15"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>772</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>772</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>775</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>775</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>775</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>779</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>785</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>788</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>788</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>788</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>788</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B73" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B83" s="15" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B85" s="15" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B86" s="15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B87" s="15" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B88" s="15" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B89" s="15" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B90" s="15" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B91" s="15" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B92" s="15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B93" s="15" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B95" s="15" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B96" s="15" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B97" s="15" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B98" s="15" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B99" s="15" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B100" s="15" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B101" s="15" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B102" s="15" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B103" s="15" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B104" s="15" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B105" s="15" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B106" s="15" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B107" s="15" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B108" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B109" s="15" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B110" s="15" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B111" s="15" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B112" s="15" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B113" s="15" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B114" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B115" s="15" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B116" s="15" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B117" s="15" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B118" s="15" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B119" s="15" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B120" s="15" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B121" s="15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B122" s="15" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B123" s="15" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B124" s="15" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B125" s="15" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B126" s="15" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B127" s="15" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B128" s="15" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B129" s="15" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B130" s="15" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B131" s="15" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B132" s="15" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B133" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B134" s="15" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B135" s="15" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B136" s="15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B137" s="15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B138" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B139" s="15" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B140" s="15" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B141" s="15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B142" s="15" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B143" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B144" s="15" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B145" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B146" s="15" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B147" s="15" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B148" s="15" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B149" s="15" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B150" s="15" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B151" s="15" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B152" s="15" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B153" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B154" s="15" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B155" s="15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B156" s="15" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B157" s="15" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B158" s="15" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B159" s="15" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B160" s="15" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B161" s="15" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B162" s="15" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B163" s="15" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B164" s="15" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B165" s="15" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B166" s="15" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B167" s="15" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B168" s="15" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B169" s="15" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B170" s="15" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B171" s="15" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B172" s="15" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B173" s="15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B174" s="15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B175" s="15" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B176" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B177" s="15" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B178" s="15" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B179" s="15" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B180" s="15" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B181" s="15" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B182" s="15" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B183" s="15" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B184" s="15" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B185" s="15" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B186" s="15" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B187" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B188" s="15" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B189" s="15" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B190" s="15" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B191" s="15" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B192" s="15" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="15" t="s">
+        <v>905</v>
+      </c>
+      <c r="B193" s="15" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B194" s="15" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B195" s="15" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B196" s="15" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B197" s="15" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B198" s="15" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B199" s="15" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B200" s="15" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B201" s="15" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B202" s="15" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B203" s="15" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B204" s="15" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B205" s="15" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B206" s="15" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B207" s="15" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B208" s="15" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B209" s="15" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B210" s="15" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B211" s="15" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B212" s="15" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B213" s="15" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B214" s="15" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B215" s="15" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B216" s="15" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B217" s="15" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B218" s="15" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B219" s="15" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B220" s="15" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B221" s="15" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B222" s="15" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B223" s="15" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B224" s="15" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B225" s="15" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B226" s="15" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B227" s="15" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B228" s="15" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B229" s="15" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B230" s="15" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B231" s="15" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B232" s="15" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B233" s="15" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B234" s="15" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B235" s="15" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B236" s="15" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B237" s="15" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B238" s="15" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" s="15" t="s">
+        <v>922</v>
+      </c>
+      <c r="B239" s="15" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" s="15" t="s">
+        <v>922</v>
+      </c>
+      <c r="B240" s="15" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" s="15" t="s">
+        <v>922</v>
+      </c>
+      <c r="B241" s="15" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="15" t="s">
+        <v>922</v>
+      </c>
+      <c r="B242" s="15" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" s="15" t="s">
+        <v>927</v>
+      </c>
+      <c r="B243" s="15" t="s">
+        <v>928</v>
+      </c>
+      <c r="C243" s="15"/>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B244" s="15" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C244" s="15"/>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" s="15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B245" s="15" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C245" s="15"/>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" s="15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B246" s="15" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C246" s="15"/>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" s="15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B247" s="15" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C247" s="15"/>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" s="15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B248" s="15" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C248" s="15"/>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" s="15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B249" s="15" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C249" s="15"/>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" s="15" t="s">
+        <v>438</v>
+      </c>
+      <c r="B250" s="15" t="s">
+        <v>441</v>
+      </c>
+      <c r="C250" s="15"/>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" s="15" t="s">
+        <v>445</v>
+      </c>
+      <c r="B251" s="15" t="s">
+        <v>448</v>
+      </c>
+      <c r="C251" s="15"/>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" s="15" t="s">
+        <v>445</v>
+      </c>
+      <c r="B252" s="15" t="s">
+        <v>452</v>
+      </c>
+      <c r="C252" s="15"/>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" s="15" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B253" s="15" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C253" s="15" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" s="15" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B254" s="15" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C254" s="15" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" s="15" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B255" s="15" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C255" s="15" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" s="15" t="s">
+        <v>930</v>
+      </c>
+      <c r="B256" s="15" t="s">
+        <v>931</v>
+      </c>
+      <c r="C256" s="15"/>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" s="15" t="s">
+        <v>930</v>
+      </c>
+      <c r="B257" s="15" t="s">
+        <v>932</v>
+      </c>
+      <c r="C257" s="15"/>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" s="15" t="s">
+        <v>930</v>
+      </c>
+      <c r="B258" s="15" t="s">
+        <v>933</v>
+      </c>
+      <c r="C258" s="15"/>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" s="15" t="s">
+        <v>930</v>
+      </c>
+      <c r="B259" s="15" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" s="15" t="s">
+        <v>930</v>
+      </c>
+      <c r="B260" s="15" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" s="15" t="s">
+        <v>930</v>
+      </c>
+      <c r="B261" s="15" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" s="15" t="s">
+        <v>930</v>
+      </c>
+      <c r="B262" s="15" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" s="15" t="s">
+        <v>930</v>
+      </c>
+      <c r="B263" s="15" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" s="15" t="s">
+        <v>930</v>
+      </c>
+      <c r="B264" s="15" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" s="15" t="s">
+        <v>930</v>
+      </c>
+      <c r="B265" s="15" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" s="15" t="s">
+        <v>930</v>
+      </c>
+      <c r="B266" s="15" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" s="15" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B267" s="15" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" s="15" t="s">
+        <v>942</v>
+      </c>
+      <c r="B268" s="15" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" s="15" t="s">
+        <v>942</v>
+      </c>
+      <c r="B269" s="15" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270" s="15" t="s">
+        <v>942</v>
+      </c>
+      <c r="B270" s="15" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" s="15" t="s">
+        <v>942</v>
+      </c>
+      <c r="B271" s="15" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" s="15" t="s">
+        <v>942</v>
+      </c>
+      <c r="B272" s="15" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" s="15" t="s">
+        <v>948</v>
+      </c>
+      <c r="B273" s="15" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" s="15" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B274" s="15" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" s="15" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B275" s="15" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="B276" s="15" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="B277" s="15" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="B278" s="15" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="B279" s="15" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="B280" s="15" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="B281" s="15" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="B282" s="15" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="B283" s="15" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="B284" s="15" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="B285" s="15" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="B286" s="15" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="B287" s="15" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="B288" s="15" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="B289" s="15" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="B290" s="15" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" s="15" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B291" s="15" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" s="15" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B292" s="15" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" s="15" t="s">
+        <v>958</v>
+      </c>
+      <c r="B293" s="15" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" s="15" t="s">
+        <v>959</v>
+      </c>
+      <c r="B294" s="15" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" s="15" t="s">
+        <v>959</v>
+      </c>
+      <c r="B295" s="15" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" s="15" t="s">
+        <v>962</v>
+      </c>
+      <c r="B296" s="15" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297" s="15" t="s">
+        <v>962</v>
+      </c>
+      <c r="B297" s="15" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298" s="15" t="s">
+        <v>962</v>
+      </c>
+      <c r="B298" s="15" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A299" s="15" t="s">
+        <v>962</v>
+      </c>
+      <c r="B299" s="15" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300" s="15" t="s">
+        <v>969</v>
+      </c>
+      <c r="B300" s="15" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A301" s="15" t="s">
+        <v>970</v>
+      </c>
+      <c r="B301" s="15" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302" s="15" t="s">
+        <v>970</v>
+      </c>
+      <c r="B302" s="15" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A303" s="15" t="s">
+        <v>970</v>
+      </c>
+      <c r="B303" s="15" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304" s="15" t="s">
+        <v>974</v>
+      </c>
+      <c r="B304" s="15" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305" s="15" t="s">
+        <v>974</v>
+      </c>
+      <c r="B305" s="15" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A306" s="15" t="s">
+        <v>974</v>
+      </c>
+      <c r="B306" s="15" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A307" s="15" t="s">
+        <v>526</v>
+      </c>
+      <c r="B307" s="15" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A308" s="15" t="s">
+        <v>526</v>
+      </c>
+      <c r="B308" s="15" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A309" s="15" t="s">
+        <v>526</v>
+      </c>
+      <c r="B309" s="15" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A310" s="15" t="s">
+        <v>526</v>
+      </c>
+      <c r="B310" s="15" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A311" s="15" t="s">
+        <v>978</v>
+      </c>
+      <c r="B311" s="15" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A312" s="15" t="s">
+        <v>978</v>
+      </c>
+      <c r="B312" s="15" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A313" s="15" t="s">
+        <v>978</v>
+      </c>
+      <c r="B313" s="15" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A314" s="15" t="s">
+        <v>978</v>
+      </c>
+      <c r="B314" s="15" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A315" s="15" t="s">
+        <v>978</v>
+      </c>
+      <c r="B315" s="15" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="B316" s="15" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="B317" s="15" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A318" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="B318" s="15" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A319" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="B319" s="15" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="B320" s="15" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="B321" s="15" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="B322" s="15" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="B323" s="15" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="B324" s="15" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" s="15" t="s">
+        <v>584</v>
+      </c>
+      <c r="B325" s="15" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" s="15" t="s">
+        <v>584</v>
+      </c>
+      <c r="B326" s="15" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327" s="15" t="s">
+        <v>584</v>
+      </c>
+      <c r="B327" s="15" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328" s="15" t="s">
+        <v>584</v>
+      </c>
+      <c r="B328" s="15" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" s="15" t="s">
+        <v>584</v>
+      </c>
+      <c r="B329" s="15" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330" s="15" t="s">
+        <v>605</v>
+      </c>
+      <c r="B330" s="15" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B331" s="15" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B332" s="15" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B333" s="15" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B334" s="15" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A335" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B335" s="15" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B336" s="15" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A337" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B337" s="15" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A338" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B338" s="15" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A339" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B339" s="15" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A340" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B340" s="15" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A341" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B341" s="15" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A342" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B342" s="15" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A343" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B343" s="15" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B344" s="15" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B345" s="15" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B346" s="15" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B347" s="15" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B348" s="15" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B349" s="15" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B350" s="15" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B351" s="15" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="B352" s="15" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353" s="15" t="s">
+        <v>648</v>
+      </c>
+      <c r="B353" s="15" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A354" s="15" t="s">
+        <v>648</v>
+      </c>
+      <c r="B354" s="15" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A355" s="15" t="s">
+        <v>659</v>
+      </c>
+      <c r="B355" s="15" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A356" s="15" t="s">
+        <v>664</v>
+      </c>
+      <c r="B356" s="15" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357" s="15" t="s">
+        <v>664</v>
+      </c>
+      <c r="B357" s="15" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358" s="15" t="s">
+        <v>664</v>
+      </c>
+      <c r="B358" s="15" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359" s="15" t="s">
+        <v>678</v>
+      </c>
+      <c r="B359" s="15" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A360" s="15" t="s">
+        <v>678</v>
+      </c>
+      <c r="B360" s="15" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A361" s="15" t="s">
+        <v>678</v>
+      </c>
+      <c r="B361" s="15" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A362" s="15" t="s">
+        <v>678</v>
+      </c>
+      <c r="B362" s="15" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A363" s="15" t="s">
+        <v>678</v>
+      </c>
+      <c r="B363" s="15" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A364" s="15" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B364" s="15" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365" s="15" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B365" s="15" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A366" s="15" t="s">
+        <v>705</v>
+      </c>
+      <c r="B366" s="15" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A367" s="15" t="s">
+        <v>705</v>
+      </c>
+      <c r="B367" s="15" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A368" s="15" t="s">
+        <v>705</v>
+      </c>
+      <c r="B368" s="15" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A369" s="15" t="s">
+        <v>705</v>
+      </c>
+      <c r="B369" s="15" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A370" s="15" t="s">
+        <v>705</v>
+      </c>
+      <c r="B370" s="15" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A371" s="15" t="s">
+        <v>705</v>
+      </c>
+      <c r="B371" s="15" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A372" s="15" t="s">
+        <v>705</v>
+      </c>
+      <c r="B372" s="15" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A373" s="15" t="s">
+        <v>705</v>
+      </c>
+      <c r="B373" s="15" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A374" s="15" t="s">
+        <v>705</v>
+      </c>
+      <c r="B374" s="15" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A375" s="15" t="s">
+        <v>705</v>
+      </c>
+      <c r="B375" s="15" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A376" s="15" t="s">
+        <v>705</v>
+      </c>
+      <c r="B376" s="15" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A377" s="15" t="s">
+        <v>730</v>
+      </c>
+      <c r="B377" s="15" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A378" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="B378" s="15" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A379" s="15" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B379" s="15" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A380" s="15" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B380" s="15" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A381" s="15" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B381" s="15" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A382" s="15" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B382" s="15" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A383" s="15" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B383" s="15" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384" s="15" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B384" s="15" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A385" s="15" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B385" s="15" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A386" s="15" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B386" s="15" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A387" s="15" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B387" s="15" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A388" s="15" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B388" s="15" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B1048574">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:B63"/>
+  <sheetViews>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C61" sqref="C4:C61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>742</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>761</v>
+      </c>
+      <c r="B7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>772</v>
+      </c>
+      <c r="B8" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>775</v>
+      </c>
+      <c r="B9" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>779</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>785</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>843</v>
+      </c>
+      <c r="B12" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>788</v>
+      </c>
+      <c r="B13" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17" s="8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B18" s="8">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B19" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B20" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="B21" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="B22" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="B23" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="B24" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="B25" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>922</v>
+      </c>
+      <c r="B26" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>927</v>
+      </c>
+      <c r="B27" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B28" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="B29" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="B30" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B31" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B32" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>930</v>
+      </c>
+      <c r="B33" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B34" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>942</v>
+      </c>
+      <c r="B35" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>948</v>
+      </c>
+      <c r="B36" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B37" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="B38" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="B39" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B40" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>958</v>
+      </c>
+      <c r="B41" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>959</v>
+      </c>
+      <c r="B42" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>962</v>
+      </c>
+      <c r="B43" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>969</v>
+      </c>
+      <c r="B44" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>970</v>
+      </c>
+      <c r="B45" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>974</v>
+      </c>
+      <c r="B46" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="B47" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>978</v>
+      </c>
+      <c r="B48" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="B49" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="B50" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="B51" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>610</v>
+      </c>
+      <c r="B52" s="8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>648</v>
+      </c>
+      <c r="B53" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="B54" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="B55" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>678</v>
+      </c>
+      <c r="B56" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B57" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>705</v>
+      </c>
+      <c r="B58" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="B59" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
+        <v>737</v>
+      </c>
+      <c r="B60" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B61" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B62" s="8"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>743</v>
+      </c>
+      <c r="B63" s="8">
+        <v>385</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C388"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -14282,10 +18033,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048574">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -14294,7 +18045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J186"/>
   <sheetViews>
@@ -19613,7 +23364,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J40"/>
   <sheetViews>
@@ -21010,7 +24761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C322"/>
   <sheetViews>
@@ -23685,7 +27436,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B50"/>
   <sheetViews>
@@ -24088,7 +27839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E113"/>
   <sheetViews>
@@ -26034,7 +29785,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B373"/>
   <sheetViews>
@@ -29037,7 +32788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -29104,509 +32855,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B63"/>
-  <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C61" sqref="C4:C61"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>742</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>761</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>772</v>
-      </c>
-      <c r="B8" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>775</v>
-      </c>
-      <c r="B9" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>779</v>
-      </c>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>785</v>
-      </c>
-      <c r="B11" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>843</v>
-      </c>
-      <c r="B12" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>788</v>
-      </c>
-      <c r="B13" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B15" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B16" s="8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B17" s="8">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="B18" s="8">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="B19" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="B20" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="B21" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>905</v>
-      </c>
-      <c r="B22" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>384</v>
-      </c>
-      <c r="B23" s="8">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>394</v>
-      </c>
-      <c r="B24" s="8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>413</v>
-      </c>
-      <c r="B25" s="8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>922</v>
-      </c>
-      <c r="B26" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>927</v>
-      </c>
-      <c r="B27" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>1038</v>
-      </c>
-      <c r="B28" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>438</v>
-      </c>
-      <c r="B29" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>445</v>
-      </c>
-      <c r="B30" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>1036</v>
-      </c>
-      <c r="B31" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>1037</v>
-      </c>
-      <c r="B32" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>930</v>
-      </c>
-      <c r="B33" s="8">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>1084</v>
-      </c>
-      <c r="B34" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>942</v>
-      </c>
-      <c r="B35" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>948</v>
-      </c>
-      <c r="B36" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>1276</v>
-      </c>
-      <c r="B37" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>456</v>
-      </c>
-      <c r="B38" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>494</v>
-      </c>
-      <c r="B39" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>1277</v>
-      </c>
-      <c r="B40" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>958</v>
-      </c>
-      <c r="B41" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>959</v>
-      </c>
-      <c r="B42" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
-        <v>962</v>
-      </c>
-      <c r="B43" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
-        <v>969</v>
-      </c>
-      <c r="B44" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>970</v>
-      </c>
-      <c r="B45" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>974</v>
-      </c>
-      <c r="B46" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>526</v>
-      </c>
-      <c r="B47" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>978</v>
-      </c>
-      <c r="B48" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>543</v>
-      </c>
-      <c r="B49" s="8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>584</v>
-      </c>
-      <c r="B50" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>605</v>
-      </c>
-      <c r="B51" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
-        <v>610</v>
-      </c>
-      <c r="B52" s="8">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
-        <v>648</v>
-      </c>
-      <c r="B53" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>659</v>
-      </c>
-      <c r="B54" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>664</v>
-      </c>
-      <c r="B55" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
-        <v>678</v>
-      </c>
-      <c r="B56" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
-        <v>1003</v>
-      </c>
-      <c r="B57" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
-        <v>705</v>
-      </c>
-      <c r="B58" s="8">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
-        <v>730</v>
-      </c>
-      <c r="B59" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
-        <v>737</v>
-      </c>
-      <c r="B60" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
-        <v>1022</v>
-      </c>
-      <c r="B61" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B62" s="8"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
-        <v>743</v>
-      </c>
-      <c r="B63" s="8">
-        <v>385</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>